<commit_message>
updated to include calculation using structure
</commit_message>
<xml_diff>
--- a/multispecific_antibodies/all_antibody_sasa_chains.xlsx
+++ b/multispecific_antibodies/all_antibody_sasa_chains.xlsx
@@ -3844,7 +3844,7 @@
         <v>231</v>
       </c>
       <c r="F33" t="n">
-        <v>25672.33</v>
+        <v>25672.32</v>
       </c>
       <c r="G33" t="n">
         <v>8.56</v>
@@ -30115,7 +30115,7 @@
         <v>9.19</v>
       </c>
       <c r="H288" t="n">
-        <v>-0.23</v>
+        <v>-0.22</v>
       </c>
       <c r="I288" t="n">
         <v>0.53</v>

</xml_diff>